<commit_message>
Priya worked on checkout page
</commit_message>
<xml_diff>
--- a/Documents/Product List V1.xlsx
+++ b/Documents/Product List V1.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Y$114</definedName>
   </definedNames>
-  <calcPr calcId="144525" iterateDelta="1E-4"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="581">
   <si>
     <t>section</t>
   </si>
@@ -736,9 +736,6 @@
   </si>
   <si>
     <t>Lemon</t>
-  </si>
-  <si>
-    <t>pouch</t>
   </si>
   <si>
     <t>Bitter Gourd</t>
@@ -1997,7 +1994,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2039,7 +2036,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2081,7 +2078,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2379,11 +2376,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AME114"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N115" sqref="N115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -2499,7 +2497,7 @@
       <c r="AMD1" s="24"/>
       <c r="AME1" s="24"/>
     </row>
-    <row r="2" spans="1:1019" s="7" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:1019" s="7" customFormat="1" ht="82.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>89</v>
       </c>
@@ -2517,10 +2515,10 @@
         <v>217</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>113</v>
@@ -2538,7 +2536,7 @@
         <v>999999</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3">
@@ -2546,7 +2544,7 @@
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>224</v>
@@ -2561,7 +2559,7 @@
         <v>224</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>226</v>
@@ -2570,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>89</v>
       </c>
@@ -2588,10 +2586,10 @@
         <v>205</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>113</v>
@@ -2609,7 +2607,7 @@
         <v>999999</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3">
@@ -2617,7 +2615,7 @@
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S3" s="6" t="s">
         <v>224</v>
@@ -2632,7 +2630,7 @@
         <v>225</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X3" s="3">
         <v>0</v>
@@ -2641,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1019" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:1019" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>89</v>
       </c>
@@ -2660,7 +2658,7 @@
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>113</v>
@@ -2678,7 +2676,7 @@
         <v>999999</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3">
@@ -2686,7 +2684,7 @@
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S4" s="6" t="s">
         <v>224</v>
@@ -2701,7 +2699,7 @@
         <v>224</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X4" s="3">
         <v>0</v>
@@ -2710,7 +2708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:1019" s="7" customFormat="1" ht="110.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:1019" s="7" customFormat="1" ht="110.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>89</v>
       </c>
@@ -2728,10 +2726,10 @@
         <v>64</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>113</v>
@@ -2757,7 +2755,7 @@
       </c>
       <c r="Q5" s="3"/>
       <c r="R5" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>224</v>
@@ -2772,7 +2770,7 @@
         <v>225</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X5" s="3">
         <v>0</v>
@@ -2781,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:1019" s="7" customFormat="1" ht="51.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:1019" s="7" customFormat="1" ht="51.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>89</v>
       </c>
@@ -2799,10 +2797,10 @@
         <v>95</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>113</v>
@@ -2828,7 +2826,7 @@
       </c>
       <c r="Q6" s="3"/>
       <c r="R6" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S6" s="6" t="s">
         <v>224</v>
@@ -2843,7 +2841,7 @@
         <v>224</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X6" s="3">
         <v>0</v>
@@ -2852,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>89</v>
       </c>
@@ -2870,10 +2868,10 @@
         <v>28</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>113</v>
@@ -2914,7 +2912,7 @@
         <v>225</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X7" s="3">
         <v>0</v>
@@ -2923,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:1019" s="7" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1019" s="7" customFormat="1" ht="95.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>89</v>
       </c>
@@ -2941,10 +2939,10 @@
         <v>96</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I8" s="4" t="s">
         <v>113</v>
@@ -2970,7 +2968,7 @@
       </c>
       <c r="Q8" s="3"/>
       <c r="R8" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S8" s="6" t="s">
         <v>224</v>
@@ -2985,7 +2983,7 @@
         <v>225</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X8" s="3">
         <v>0</v>
@@ -2994,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>89</v>
       </c>
@@ -3012,10 +3010,10 @@
         <v>218</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>113</v>
@@ -3041,7 +3039,7 @@
       </c>
       <c r="Q9" s="3"/>
       <c r="R9" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>224</v>
@@ -3056,7 +3054,7 @@
         <v>225</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X9" s="3">
         <v>0</v>
@@ -3065,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:1019" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:1019" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>89</v>
       </c>
@@ -3083,10 +3081,10 @@
         <v>207</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>113</v>
@@ -3112,7 +3110,7 @@
       </c>
       <c r="Q10" s="3"/>
       <c r="R10" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>224</v>
@@ -3127,7 +3125,7 @@
         <v>225</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X10" s="3">
         <v>0</v>
@@ -3136,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:1019" ht="63" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:1019" ht="63" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>89</v>
       </c>
@@ -3154,10 +3152,10 @@
         <v>97</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I11" s="4" t="s">
         <v>113</v>
@@ -3183,7 +3181,7 @@
       </c>
       <c r="Q11" s="3"/>
       <c r="R11" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="S11" s="6" t="s">
         <v>224</v>
@@ -3198,7 +3196,7 @@
         <v>224</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X11" s="3">
         <v>0</v>
@@ -3207,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>89</v>
       </c>
@@ -3225,10 +3223,10 @@
         <v>31</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>113</v>
@@ -3254,7 +3252,7 @@
       </c>
       <c r="Q12" s="3"/>
       <c r="R12" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S12" s="6" t="s">
         <v>224</v>
@@ -3269,7 +3267,7 @@
         <v>225</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X12" s="3">
         <v>0</v>
@@ -3278,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:1019" s="7" customFormat="1" ht="51.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:1019" s="7" customFormat="1" ht="51.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>89</v>
       </c>
@@ -3296,10 +3294,10 @@
         <v>98</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I13" s="4" t="s">
         <v>113</v>
@@ -3325,7 +3323,7 @@
       </c>
       <c r="Q13" s="3"/>
       <c r="R13" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="S13" s="6" t="s">
         <v>224</v>
@@ -3340,7 +3338,7 @@
         <v>225</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X13" s="3">
         <v>0</v>
@@ -3349,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:1019" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:1019" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>89</v>
       </c>
@@ -3367,10 +3365,10 @@
         <v>27</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>113</v>
@@ -3396,7 +3394,7 @@
       </c>
       <c r="Q14" s="3"/>
       <c r="R14" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S14" s="6" t="s">
         <v>224</v>
@@ -3411,7 +3409,7 @@
         <v>224</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X14" s="3">
         <v>0</v>
@@ -3420,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>89</v>
       </c>
@@ -3438,10 +3436,10 @@
         <v>32</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>113</v>
@@ -3467,7 +3465,7 @@
       </c>
       <c r="Q15" s="3"/>
       <c r="R15" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="S15" s="6" t="s">
         <v>224</v>
@@ -3482,7 +3480,7 @@
         <v>225</v>
       </c>
       <c r="W15" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X15" s="3">
         <v>0</v>
@@ -3491,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:1019" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:1019" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>89</v>
       </c>
@@ -3509,10 +3507,10 @@
         <v>29</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>113</v>
@@ -3530,7 +3528,7 @@
         <v>999999</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3">
@@ -3538,7 +3536,7 @@
       </c>
       <c r="Q16" s="3"/>
       <c r="R16" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S16" s="6" t="s">
         <v>224</v>
@@ -3553,7 +3551,7 @@
         <v>224</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X16" s="3">
         <v>0</v>
@@ -3562,7 +3560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>89</v>
       </c>
@@ -3580,10 +3578,10 @@
         <v>30</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>113</v>
@@ -3609,7 +3607,7 @@
       </c>
       <c r="Q17" s="3"/>
       <c r="R17" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="S17" s="6" t="s">
         <v>224</v>
@@ -3624,7 +3622,7 @@
         <v>225</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X17" s="3">
         <v>0</v>
@@ -3633,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
@@ -3651,10 +3649,10 @@
         <v>219</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>113</v>
@@ -3672,7 +3670,7 @@
         <v>999999</v>
       </c>
       <c r="N18" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3">
@@ -3680,7 +3678,7 @@
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="S18" s="6" t="s">
         <v>224</v>
@@ -3695,7 +3693,7 @@
         <v>224</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X18" s="3">
         <v>0</v>
@@ -3704,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>89</v>
       </c>
@@ -3719,13 +3717,13 @@
         <v>2111</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>113</v>
@@ -3743,7 +3741,7 @@
         <v>999999</v>
       </c>
       <c r="N19" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O19" s="3"/>
       <c r="P19" s="3">
@@ -3751,7 +3749,7 @@
       </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="S19" s="3" t="s">
         <v>224</v>
@@ -3766,7 +3764,7 @@
         <v>225</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X19" s="3">
         <v>0</v>
@@ -3775,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
         <v>89</v>
       </c>
@@ -3793,10 +3791,10 @@
         <v>99</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>113</v>
@@ -3814,7 +3812,7 @@
         <v>999999</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O20" s="3"/>
       <c r="P20" s="3">
@@ -3822,7 +3820,7 @@
       </c>
       <c r="Q20" s="3"/>
       <c r="R20" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S20" s="6" t="s">
         <v>224</v>
@@ -3837,7 +3835,7 @@
         <v>225</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X20" s="3">
         <v>0</v>
@@ -3846,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>89</v>
       </c>
@@ -3864,10 +3862,10 @@
         <v>100</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H21" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>113</v>
@@ -3885,7 +3883,7 @@
         <v>999999</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3">
@@ -3893,7 +3891,7 @@
       </c>
       <c r="Q21" s="3"/>
       <c r="R21" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="S21" s="6" t="s">
         <v>224</v>
@@ -3908,7 +3906,7 @@
         <v>225</v>
       </c>
       <c r="W21" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X21" s="3">
         <v>0</v>
@@ -3917,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
         <v>89</v>
       </c>
@@ -3935,10 +3933,10 @@
         <v>101</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>113</v>
@@ -3964,7 +3962,7 @@
       </c>
       <c r="Q22" s="3"/>
       <c r="R22" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S22" s="6" t="s">
         <v>224</v>
@@ -3979,7 +3977,7 @@
         <v>225</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X22" s="3">
         <v>0</v>
@@ -3988,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
         <v>89</v>
       </c>
@@ -4006,10 +4004,10 @@
         <v>107</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>113</v>
@@ -4027,7 +4025,7 @@
         <v>999999</v>
       </c>
       <c r="N23" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3">
@@ -4035,7 +4033,7 @@
       </c>
       <c r="Q23" s="3"/>
       <c r="R23" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="S23" s="6" t="s">
         <v>224</v>
@@ -4050,7 +4048,7 @@
         <v>225</v>
       </c>
       <c r="W23" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X23" s="3">
         <v>0</v>
@@ -4059,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3" t="s">
         <v>89</v>
       </c>
@@ -4077,10 +4075,10 @@
         <v>108</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>113</v>
@@ -4106,7 +4104,7 @@
       </c>
       <c r="Q24" s="3"/>
       <c r="R24" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="S24" s="6" t="s">
         <v>224</v>
@@ -4121,7 +4119,7 @@
         <v>225</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X24" s="3">
         <v>0</v>
@@ -4130,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -4148,10 +4146,10 @@
         <v>102</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>113</v>
@@ -4177,7 +4175,7 @@
       </c>
       <c r="Q25" s="3"/>
       <c r="R25" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="S25" s="6" t="s">
         <v>224</v>
@@ -4192,7 +4190,7 @@
         <v>225</v>
       </c>
       <c r="W25" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X25" s="3">
         <v>0</v>
@@ -4201,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3" t="s">
         <v>89</v>
       </c>
@@ -4219,10 +4217,10 @@
         <v>103</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>113</v>
@@ -4248,7 +4246,7 @@
       </c>
       <c r="Q26" s="3"/>
       <c r="R26" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="S26" s="6" t="s">
         <v>224</v>
@@ -4263,7 +4261,7 @@
         <v>225</v>
       </c>
       <c r="W26" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X26" s="3">
         <v>0</v>
@@ -4272,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="7" customFormat="1" ht="114.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3" t="s">
         <v>89</v>
       </c>
@@ -4290,10 +4288,10 @@
         <v>104</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>113</v>
@@ -4319,7 +4317,7 @@
       </c>
       <c r="Q27" s="3"/>
       <c r="R27" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S27" s="6" t="s">
         <v>224</v>
@@ -4334,7 +4332,7 @@
         <v>225</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X27" s="3">
         <v>0</v>
@@ -4343,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3" t="s">
         <v>89</v>
       </c>
@@ -4358,13 +4356,13 @@
         <v>2200</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>113</v>
@@ -4390,7 +4388,7 @@
       </c>
       <c r="Q28" s="3"/>
       <c r="R28" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="S28" s="6" t="s">
         <v>224</v>
@@ -4405,7 +4403,7 @@
         <v>224</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X28" s="3">
         <v>0</v>
@@ -4414,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3" t="s">
         <v>89</v>
       </c>
@@ -4429,13 +4427,13 @@
         <v>2210</v>
       </c>
       <c r="F29" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="G29" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>284</v>
-      </c>
       <c r="H29" s="13" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>113</v>
@@ -4461,7 +4459,7 @@
       </c>
       <c r="Q29" s="3"/>
       <c r="R29" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="S29" s="6" t="s">
         <v>224</v>
@@ -4476,7 +4474,7 @@
         <v>225</v>
       </c>
       <c r="W29" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X29" s="3">
         <v>0</v>
@@ -4485,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
@@ -4503,10 +4501,10 @@
         <v>109</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>113</v>
@@ -4524,7 +4522,7 @@
         <v>999999</v>
       </c>
       <c r="N30" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3">
@@ -4532,7 +4530,7 @@
       </c>
       <c r="Q30" s="3"/>
       <c r="R30" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="S30" s="6" t="s">
         <v>224</v>
@@ -4547,7 +4545,7 @@
         <v>225</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X30" s="3">
         <v>0</v>
@@ -4556,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3" t="s">
         <v>89</v>
       </c>
@@ -4571,13 +4569,13 @@
         <v>2221</v>
       </c>
       <c r="F31" s="15" t="s">
+        <v>544</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="H31" s="10" t="s">
         <v>545</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>546</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>113</v>
@@ -4595,7 +4593,7 @@
         <v>999999</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3">
@@ -4603,7 +4601,7 @@
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="S31" s="6" t="s">
         <v>224</v>
@@ -4618,7 +4616,7 @@
         <v>225</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X31" s="3">
         <v>0</v>
@@ -4627,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3" t="s">
         <v>89</v>
       </c>
@@ -4645,10 +4643,10 @@
         <v>110</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>113</v>
@@ -4674,7 +4672,7 @@
       </c>
       <c r="Q32" s="3"/>
       <c r="R32" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S32" s="6" t="s">
         <v>224</v>
@@ -4689,7 +4687,7 @@
         <v>225</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X32" s="3">
         <v>0</v>
@@ -4698,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3" t="s">
         <v>89</v>
       </c>
@@ -4707,19 +4705,19 @@
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E33" s="4">
         <v>2240</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>113</v>
@@ -4745,7 +4743,7 @@
       </c>
       <c r="Q33" s="3"/>
       <c r="R33" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S33" s="6" t="s">
         <v>224</v>
@@ -4760,7 +4758,7 @@
         <v>225</v>
       </c>
       <c r="W33" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X33" s="3">
         <v>0</v>
@@ -4769,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -4787,10 +4785,10 @@
         <v>208</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>113</v>
@@ -4816,7 +4814,7 @@
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S34" s="6" t="s">
         <v>224</v>
@@ -4831,7 +4829,7 @@
         <v>225</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X34" s="3">
         <v>0</v>
@@ -4840,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:25" s="7" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:25" s="7" customFormat="1" ht="87" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3" t="s">
         <v>84</v>
       </c>
@@ -4858,10 +4856,10 @@
         <v>209</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>113</v>
@@ -4887,7 +4885,7 @@
       </c>
       <c r="Q35" s="3"/>
       <c r="R35" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S35" s="6" t="s">
         <v>224</v>
@@ -4902,7 +4900,7 @@
         <v>225</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X35" s="3">
         <v>0</v>
@@ -4911,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="7" customFormat="1" ht="110.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:25" s="7" customFormat="1" ht="110.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3" t="s">
         <v>84</v>
       </c>
@@ -4929,10 +4927,10 @@
         <v>33</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>113</v>
@@ -4958,7 +4956,7 @@
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S36" s="6" t="s">
         <v>224</v>
@@ -4973,7 +4971,7 @@
         <v>225</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X36" s="3">
         <v>0</v>
@@ -4982,7 +4980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:25" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3" t="s">
         <v>84</v>
       </c>
@@ -5001,7 +4999,7 @@
       </c>
       <c r="G37" s="19"/>
       <c r="H37" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I37" s="4" t="s">
         <v>113</v>
@@ -5027,7 +5025,7 @@
       </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="S37" s="6" t="s">
         <v>224</v>
@@ -5042,7 +5040,7 @@
         <v>225</v>
       </c>
       <c r="W37" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X37" s="3">
         <v>0</v>
@@ -5051,7 +5049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3" t="s">
         <v>84</v>
       </c>
@@ -5069,10 +5067,10 @@
         <v>220</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I38" s="4" t="s">
         <v>113</v>
@@ -5098,7 +5096,7 @@
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="S38" s="6" t="s">
         <v>224</v>
@@ -5113,7 +5111,7 @@
         <v>225</v>
       </c>
       <c r="W38" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X38" s="3">
         <v>0</v>
@@ -5122,7 +5120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3" t="s">
         <v>84</v>
       </c>
@@ -5140,10 +5138,10 @@
         <v>210</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H39" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I39" s="4" t="s">
         <v>113</v>
@@ -5169,7 +5167,7 @@
       </c>
       <c r="Q39" s="3"/>
       <c r="R39" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S39" s="6" t="s">
         <v>224</v>
@@ -5184,7 +5182,7 @@
         <v>225</v>
       </c>
       <c r="W39" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X39" s="3">
         <v>0</v>
@@ -5193,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3" t="s">
         <v>84</v>
       </c>
@@ -5211,10 +5209,10 @@
         <v>211</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H40" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I40" s="4" t="s">
         <v>113</v>
@@ -5240,7 +5238,7 @@
       </c>
       <c r="Q40" s="3"/>
       <c r="R40" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="S40" s="6" t="s">
         <v>224</v>
@@ -5255,7 +5253,7 @@
         <v>225</v>
       </c>
       <c r="W40" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X40" s="3">
         <v>0</v>
@@ -5264,7 +5262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
@@ -5282,10 +5280,10 @@
         <v>35</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H41" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>113</v>
@@ -5311,7 +5309,7 @@
       </c>
       <c r="Q41" s="3"/>
       <c r="R41" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="S41" s="6" t="s">
         <v>224</v>
@@ -5326,7 +5324,7 @@
         <v>225</v>
       </c>
       <c r="W41" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X41" s="3">
         <v>0</v>
@@ -5335,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:25" s="7" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3" t="s">
         <v>84</v>
       </c>
@@ -5353,10 +5351,10 @@
         <v>36</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I42" s="4" t="s">
         <v>113</v>
@@ -5382,7 +5380,7 @@
       </c>
       <c r="Q42" s="3"/>
       <c r="R42" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="S42" s="6" t="s">
         <v>224</v>
@@ -5397,7 +5395,7 @@
         <v>224</v>
       </c>
       <c r="W42" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X42" s="3">
         <v>0</v>
@@ -5406,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="130.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:25" ht="130.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3" t="s">
         <v>84</v>
       </c>
@@ -5424,10 +5422,10 @@
         <v>37</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H43" s="10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I43" s="4" t="s">
         <v>113</v>
@@ -5453,7 +5451,7 @@
       </c>
       <c r="Q43" s="3"/>
       <c r="R43" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="S43" s="6" t="s">
         <v>224</v>
@@ -5468,7 +5466,7 @@
         <v>225</v>
       </c>
       <c r="W43" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X43" s="3">
         <v>0</v>
@@ -5477,7 +5475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3" t="s">
         <v>84</v>
       </c>
@@ -5495,10 +5493,10 @@
         <v>38</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H44" s="10" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I44" s="4" t="s">
         <v>113</v>
@@ -5524,7 +5522,7 @@
       </c>
       <c r="Q44" s="3"/>
       <c r="R44" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="S44" s="6" t="s">
         <v>224</v>
@@ -5539,7 +5537,7 @@
         <v>225</v>
       </c>
       <c r="W44" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X44" s="3">
         <v>0</v>
@@ -5548,7 +5546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3" t="s">
         <v>84</v>
       </c>
@@ -5566,10 +5564,10 @@
         <v>39</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I45" s="4" t="s">
         <v>113</v>
@@ -5595,7 +5593,7 @@
       </c>
       <c r="Q45" s="3"/>
       <c r="R45" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S45" s="6" t="s">
         <v>224</v>
@@ -5610,7 +5608,7 @@
         <v>225</v>
       </c>
       <c r="W45" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X45" s="3">
         <v>0</v>
@@ -5619,7 +5617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:25" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3" t="s">
         <v>84</v>
       </c>
@@ -5637,10 +5635,10 @@
         <v>40</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H46" s="10" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I46" s="4" t="s">
         <v>113</v>
@@ -5666,7 +5664,7 @@
       </c>
       <c r="Q46" s="3"/>
       <c r="R46" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="S46" s="6" t="s">
         <v>224</v>
@@ -5681,7 +5679,7 @@
         <v>225</v>
       </c>
       <c r="W46" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X46" s="3">
         <v>0</v>
@@ -5690,7 +5688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3" t="s">
         <v>84</v>
       </c>
@@ -5708,10 +5706,10 @@
         <v>41</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H47" s="10" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I47" s="4" t="s">
         <v>113</v>
@@ -5737,7 +5735,7 @@
       </c>
       <c r="Q47" s="3"/>
       <c r="R47" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="S47" s="6" t="s">
         <v>224</v>
@@ -5752,7 +5750,7 @@
         <v>225</v>
       </c>
       <c r="W47" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X47" s="3">
         <v>0</v>
@@ -5761,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3" t="s">
         <v>84</v>
       </c>
@@ -5779,10 +5777,10 @@
         <v>42</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>113</v>
@@ -5808,7 +5806,7 @@
       </c>
       <c r="Q48" s="3"/>
       <c r="R48" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="S48" s="6" t="s">
         <v>224</v>
@@ -5823,7 +5821,7 @@
         <v>225</v>
       </c>
       <c r="W48" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X48" s="3">
         <v>0</v>
@@ -5832,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3" t="s">
         <v>84</v>
       </c>
@@ -5850,10 +5848,10 @@
         <v>43</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>113</v>
@@ -5879,7 +5877,7 @@
       </c>
       <c r="Q49" s="3"/>
       <c r="R49" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S49" s="6" t="s">
         <v>224</v>
@@ -5894,7 +5892,7 @@
         <v>225</v>
       </c>
       <c r="W49" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X49" s="3">
         <v>0</v>
@@ -5903,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3" t="s">
         <v>84</v>
       </c>
@@ -5921,10 +5919,10 @@
         <v>44</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I50" s="4" t="s">
         <v>113</v>
@@ -5950,7 +5948,7 @@
       </c>
       <c r="Q50" s="3"/>
       <c r="R50" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S50" s="6" t="s">
         <v>224</v>
@@ -5965,7 +5963,7 @@
         <v>225</v>
       </c>
       <c r="W50" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X50" s="3">
         <v>0</v>
@@ -5974,7 +5972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3" t="s">
         <v>84</v>
       </c>
@@ -5992,10 +5990,10 @@
         <v>45</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>113</v>
@@ -6021,7 +6019,7 @@
       </c>
       <c r="Q51" s="3"/>
       <c r="R51" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="S51" s="6" t="s">
         <v>224</v>
@@ -6036,7 +6034,7 @@
         <v>224</v>
       </c>
       <c r="W51" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X51" s="3">
         <v>0</v>
@@ -6045,7 +6043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3" t="s">
         <v>84</v>
       </c>
@@ -6063,10 +6061,10 @@
         <v>46</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>113</v>
@@ -6092,7 +6090,7 @@
       </c>
       <c r="Q52" s="3"/>
       <c r="R52" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S52" s="6" t="s">
         <v>224</v>
@@ -6107,7 +6105,7 @@
         <v>225</v>
       </c>
       <c r="W52" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X52" s="3">
         <v>0</v>
@@ -6116,7 +6114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3" t="s">
         <v>84</v>
       </c>
@@ -6134,10 +6132,10 @@
         <v>47</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>113</v>
@@ -6163,7 +6161,7 @@
       </c>
       <c r="Q53" s="3"/>
       <c r="R53" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S53" s="6" t="s">
         <v>224</v>
@@ -6178,7 +6176,7 @@
         <v>225</v>
       </c>
       <c r="W53" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X53" s="3">
         <v>0</v>
@@ -6187,7 +6185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3" t="s">
         <v>84</v>
       </c>
@@ -6205,10 +6203,10 @@
         <v>48</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>113</v>
@@ -6234,7 +6232,7 @@
       </c>
       <c r="Q54" s="3"/>
       <c r="R54" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="S54" s="6" t="s">
         <v>224</v>
@@ -6249,7 +6247,7 @@
         <v>225</v>
       </c>
       <c r="W54" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X54" s="3">
         <v>0</v>
@@ -6258,7 +6256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3" t="s">
         <v>84</v>
       </c>
@@ -6276,10 +6274,10 @@
         <v>49</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>113</v>
@@ -6305,7 +6303,7 @@
       </c>
       <c r="Q55" s="3"/>
       <c r="R55" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="S55" s="6" t="s">
         <v>224</v>
@@ -6320,7 +6318,7 @@
         <v>225</v>
       </c>
       <c r="W55" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X55" s="3">
         <v>0</v>
@@ -6329,7 +6327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3" t="s">
         <v>84</v>
       </c>
@@ -6347,10 +6345,10 @@
         <v>50</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I56" s="4" t="s">
         <v>113</v>
@@ -6376,7 +6374,7 @@
       </c>
       <c r="Q56" s="3"/>
       <c r="R56" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="S56" s="6" t="s">
         <v>224</v>
@@ -6391,7 +6389,7 @@
         <v>225</v>
       </c>
       <c r="W56" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X56" s="3">
         <v>0</v>
@@ -6400,7 +6398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:25" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:25" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3" t="s">
         <v>84</v>
       </c>
@@ -6418,10 +6416,10 @@
         <v>51</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>113</v>
@@ -6447,7 +6445,7 @@
       </c>
       <c r="Q57" s="3"/>
       <c r="R57" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S57" s="6" t="s">
         <v>224</v>
@@ -6462,7 +6460,7 @@
         <v>225</v>
       </c>
       <c r="W57" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X57" s="3">
         <v>0</v>
@@ -6471,7 +6469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3" t="s">
         <v>84</v>
       </c>
@@ -6489,10 +6487,10 @@
         <v>52</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>113</v>
@@ -6518,7 +6516,7 @@
       </c>
       <c r="Q58" s="3"/>
       <c r="R58" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S58" s="6" t="s">
         <v>224</v>
@@ -6533,7 +6531,7 @@
         <v>224</v>
       </c>
       <c r="W58" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X58" s="3">
         <v>0</v>
@@ -6542,7 +6540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3" t="s">
         <v>84</v>
       </c>
@@ -6557,13 +6555,13 @@
         <v>3181</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G59" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H59" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>113</v>
@@ -6589,7 +6587,7 @@
       </c>
       <c r="Q59" s="3"/>
       <c r="R59" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S59" s="6" t="s">
         <v>224</v>
@@ -6604,7 +6602,7 @@
         <v>225</v>
       </c>
       <c r="W59" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X59" s="3">
         <v>0</v>
@@ -6613,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3" t="s">
         <v>84</v>
       </c>
@@ -6631,10 +6629,10 @@
         <v>53</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I60" s="4" t="s">
         <v>113</v>
@@ -6660,7 +6658,7 @@
       </c>
       <c r="Q60" s="3"/>
       <c r="R60" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S60" s="6" t="s">
         <v>224</v>
@@ -6675,7 +6673,7 @@
         <v>225</v>
       </c>
       <c r="W60" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X60" s="3">
         <v>0</v>
@@ -6684,7 +6682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:25" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:25" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3" t="s">
         <v>84</v>
       </c>
@@ -6702,10 +6700,10 @@
         <v>54</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>113</v>
@@ -6731,7 +6729,7 @@
       </c>
       <c r="Q61" s="3"/>
       <c r="R61" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="S61" s="6" t="s">
         <v>224</v>
@@ -6746,7 +6744,7 @@
         <v>225</v>
       </c>
       <c r="W61" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X61" s="3">
         <v>0</v>
@@ -6755,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3" t="s">
         <v>84</v>
       </c>
@@ -6770,13 +6768,13 @@
         <v>3210</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I62" s="4" t="s">
         <v>113</v>
@@ -6802,7 +6800,7 @@
       </c>
       <c r="Q62" s="3"/>
       <c r="R62" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="S62" s="6" t="s">
         <v>224</v>
@@ -6817,7 +6815,7 @@
         <v>225</v>
       </c>
       <c r="W62" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X62" s="3">
         <v>0</v>
@@ -6826,7 +6824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:25" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:25" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3" t="s">
         <v>84</v>
       </c>
@@ -6844,10 +6842,10 @@
         <v>55</v>
       </c>
       <c r="G63" s="8" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H63" s="10" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>113</v>
@@ -6873,7 +6871,7 @@
       </c>
       <c r="Q63" s="3"/>
       <c r="R63" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="S63" s="6" t="s">
         <v>224</v>
@@ -6888,7 +6886,7 @@
         <v>225</v>
       </c>
       <c r="W63" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X63" s="3">
         <v>0</v>
@@ -6897,7 +6895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:25" ht="78.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:25" ht="78.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3" t="s">
         <v>84</v>
       </c>
@@ -6915,10 +6913,10 @@
         <v>56</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H64" s="10" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I64" s="4" t="s">
         <v>113</v>
@@ -6944,7 +6942,7 @@
       </c>
       <c r="Q64" s="3"/>
       <c r="R64" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="S64" s="6" t="s">
         <v>224</v>
@@ -6959,7 +6957,7 @@
         <v>225</v>
       </c>
       <c r="W64" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X64" s="3">
         <v>0</v>
@@ -6968,7 +6966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:25" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:25" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3" t="s">
         <v>84</v>
       </c>
@@ -6986,10 +6984,10 @@
         <v>57</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H65" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>113</v>
@@ -7015,7 +7013,7 @@
       </c>
       <c r="Q65" s="3"/>
       <c r="R65" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="S65" s="6" t="s">
         <v>224</v>
@@ -7030,7 +7028,7 @@
         <v>225</v>
       </c>
       <c r="W65" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X65" s="3">
         <v>0</v>
@@ -7039,7 +7037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3" t="s">
         <v>84</v>
       </c>
@@ -7057,10 +7055,10 @@
         <v>58</v>
       </c>
       <c r="G66" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>113</v>
@@ -7086,7 +7084,7 @@
       </c>
       <c r="Q66" s="3"/>
       <c r="R66" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="S66" s="6" t="s">
         <v>224</v>
@@ -7101,7 +7099,7 @@
         <v>225</v>
       </c>
       <c r="W66" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X66" s="3">
         <v>0</v>
@@ -7110,7 +7108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:25" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:25" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3" t="s">
         <v>84</v>
       </c>
@@ -7128,10 +7126,10 @@
         <v>59</v>
       </c>
       <c r="G67" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>113</v>
@@ -7157,7 +7155,7 @@
       </c>
       <c r="Q67" s="3"/>
       <c r="R67" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="S67" s="6" t="s">
         <v>224</v>
@@ -7172,7 +7170,7 @@
         <v>225</v>
       </c>
       <c r="W67" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X67" s="3">
         <v>0</v>
@@ -7181,7 +7179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:25" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:25" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3" t="s">
         <v>84</v>
       </c>
@@ -7199,10 +7197,10 @@
         <v>60</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H68" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I68" s="4" t="s">
         <v>113</v>
@@ -7228,7 +7226,7 @@
       </c>
       <c r="Q68" s="3"/>
       <c r="R68" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="S68" s="6" t="s">
         <v>224</v>
@@ -7243,7 +7241,7 @@
         <v>225</v>
       </c>
       <c r="W68" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X68" s="3">
         <v>0</v>
@@ -7252,7 +7250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3" t="s">
         <v>84</v>
       </c>
@@ -7270,10 +7268,10 @@
         <v>61</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H69" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>113</v>
@@ -7299,7 +7297,7 @@
       </c>
       <c r="Q69" s="3"/>
       <c r="R69" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="S69" s="6" t="s">
         <v>224</v>
@@ -7314,7 +7312,7 @@
         <v>225</v>
       </c>
       <c r="W69" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X69" s="3">
         <v>0</v>
@@ -7323,7 +7321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:25" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:25" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3" t="s">
         <v>84</v>
       </c>
@@ -7341,10 +7339,10 @@
         <v>62</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I70" s="4" t="s">
         <v>113</v>
@@ -7370,7 +7368,7 @@
       </c>
       <c r="Q70" s="3"/>
       <c r="R70" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="S70" s="6" t="s">
         <v>224</v>
@@ -7385,7 +7383,7 @@
         <v>225</v>
       </c>
       <c r="W70" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X70" s="3">
         <v>0</v>
@@ -7394,7 +7392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3" t="s">
         <v>84</v>
       </c>
@@ -7412,10 +7410,10 @@
         <v>63</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H71" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I71" s="4" t="s">
         <v>113</v>
@@ -7441,7 +7439,7 @@
       </c>
       <c r="Q71" s="3"/>
       <c r="R71" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="S71" s="6" t="s">
         <v>224</v>
@@ -7456,7 +7454,7 @@
         <v>225</v>
       </c>
       <c r="W71" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X71" s="3">
         <v>0</v>
@@ -7483,10 +7481,10 @@
         <v>235</v>
       </c>
       <c r="G72" s="8" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H72" s="10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>113</v>
@@ -7504,7 +7502,7 @@
         <v>999999</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O72" s="3"/>
       <c r="P72" s="3">
@@ -7512,7 +7510,7 @@
       </c>
       <c r="Q72" s="3"/>
       <c r="R72" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="S72" s="6" t="s">
         <v>224</v>
@@ -7527,7 +7525,7 @@
         <v>225</v>
       </c>
       <c r="W72" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X72" s="3">
         <v>0</v>
@@ -7536,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="3" t="s">
         <v>84</v>
       </c>
@@ -7554,10 +7552,10 @@
         <v>65</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H73" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>113</v>
@@ -7583,7 +7581,7 @@
       </c>
       <c r="Q73" s="3"/>
       <c r="R73" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="S73" s="6" t="s">
         <v>224</v>
@@ -7598,7 +7596,7 @@
         <v>225</v>
       </c>
       <c r="W73" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X73" s="3">
         <v>0</v>
@@ -7607,7 +7605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="3" t="s">
         <v>84</v>
       </c>
@@ -7625,10 +7623,10 @@
         <v>66</v>
       </c>
       <c r="G74" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I74" s="4" t="s">
         <v>113</v>
@@ -7654,7 +7652,7 @@
       </c>
       <c r="Q74" s="3"/>
       <c r="R74" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="S74" s="6" t="s">
         <v>224</v>
@@ -7669,7 +7667,7 @@
         <v>225</v>
       </c>
       <c r="W74" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X74" s="3">
         <v>0</v>
@@ -7678,7 +7676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="3" t="s">
         <v>84</v>
       </c>
@@ -7696,10 +7694,10 @@
         <v>67</v>
       </c>
       <c r="G75" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I75" s="4" t="s">
         <v>113</v>
@@ -7725,7 +7723,7 @@
       </c>
       <c r="Q75" s="3"/>
       <c r="R75" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="S75" s="6" t="s">
         <v>224</v>
@@ -7740,7 +7738,7 @@
         <v>225</v>
       </c>
       <c r="W75" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X75" s="3">
         <v>0</v>
@@ -7749,7 +7747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:25" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:25" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="3" t="s">
         <v>84</v>
       </c>
@@ -7767,10 +7765,10 @@
         <v>68</v>
       </c>
       <c r="G76" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H76" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I76" s="4" t="s">
         <v>113</v>
@@ -7796,7 +7794,7 @@
       </c>
       <c r="Q76" s="3"/>
       <c r="R76" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="S76" s="6" t="s">
         <v>224</v>
@@ -7811,7 +7809,7 @@
         <v>225</v>
       </c>
       <c r="W76" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X76" s="3">
         <v>0</v>
@@ -7820,7 +7818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:25" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:25" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="3" t="s">
         <v>84</v>
       </c>
@@ -7838,10 +7836,10 @@
         <v>69</v>
       </c>
       <c r="G77" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H77" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I77" s="4" t="s">
         <v>113</v>
@@ -7867,7 +7865,7 @@
       </c>
       <c r="Q77" s="3"/>
       <c r="R77" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="S77" s="6" t="s">
         <v>224</v>
@@ -7882,7 +7880,7 @@
         <v>225</v>
       </c>
       <c r="W77" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X77" s="3">
         <v>0</v>
@@ -7891,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="3" t="s">
         <v>84</v>
       </c>
@@ -7909,10 +7907,10 @@
         <v>70</v>
       </c>
       <c r="G78" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I78" s="4" t="s">
         <v>113</v>
@@ -7938,7 +7936,7 @@
       </c>
       <c r="Q78" s="3"/>
       <c r="R78" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="S78" s="6" t="s">
         <v>224</v>
@@ -7953,7 +7951,7 @@
         <v>225</v>
       </c>
       <c r="W78" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X78" s="3">
         <v>0</v>
@@ -7962,7 +7960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="3" t="s">
         <v>84</v>
       </c>
@@ -7980,10 +7978,10 @@
         <v>71</v>
       </c>
       <c r="G79" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H79" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I79" s="4" t="s">
         <v>113</v>
@@ -8009,7 +8007,7 @@
       </c>
       <c r="Q79" s="3"/>
       <c r="R79" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="S79" s="6" t="s">
         <v>224</v>
@@ -8024,7 +8022,7 @@
         <v>225</v>
       </c>
       <c r="W79" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X79" s="3">
         <v>0</v>
@@ -8033,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:25" s="7" customFormat="1" ht="78.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:25" s="7" customFormat="1" ht="78.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="3" t="s">
         <v>84</v>
       </c>
@@ -8051,10 +8049,10 @@
         <v>72</v>
       </c>
       <c r="G80" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="I80" s="4" t="s">
         <v>113</v>
@@ -8080,7 +8078,7 @@
       </c>
       <c r="Q80" s="3"/>
       <c r="R80" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="S80" s="6" t="s">
         <v>224</v>
@@ -8095,7 +8093,7 @@
         <v>225</v>
       </c>
       <c r="W80" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X80" s="3">
         <v>0</v>
@@ -8104,7 +8102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:1019" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:1019" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="3" t="s">
         <v>84</v>
       </c>
@@ -8119,13 +8117,13 @@
         <v>3400</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G81" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H81" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I81" s="4" t="s">
         <v>113</v>
@@ -8151,7 +8149,7 @@
       </c>
       <c r="Q81" s="3"/>
       <c r="R81" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="S81" s="6" t="s">
         <v>224</v>
@@ -8166,7 +8164,7 @@
         <v>225</v>
       </c>
       <c r="W81" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X81" s="3">
         <v>0</v>
@@ -8175,7 +8173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:1019" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:1019" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="3" t="s">
         <v>84</v>
       </c>
@@ -8193,10 +8191,10 @@
         <v>230</v>
       </c>
       <c r="G82" s="8" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H82" s="10" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I82" s="4" t="s">
         <v>113</v>
@@ -8222,7 +8220,7 @@
       </c>
       <c r="Q82" s="3"/>
       <c r="R82" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="S82" s="6" t="s">
         <v>224</v>
@@ -8237,7 +8235,7 @@
         <v>225</v>
       </c>
       <c r="W82" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X82" s="3">
         <v>0</v>
@@ -8246,7 +8244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:1019" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:1019" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="3" t="s">
         <v>84</v>
       </c>
@@ -8264,10 +8262,10 @@
         <v>214</v>
       </c>
       <c r="G83" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H83" s="10" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="I83" s="4" t="s">
         <v>113</v>
@@ -8293,7 +8291,7 @@
       </c>
       <c r="Q83" s="3"/>
       <c r="R83" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="S83" s="6" t="s">
         <v>224</v>
@@ -8308,7 +8306,7 @@
         <v>225</v>
       </c>
       <c r="W83" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X83" s="3">
         <v>0</v>
@@ -8317,7 +8315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:1019" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:1019" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="3" t="s">
         <v>84</v>
       </c>
@@ -8326,7 +8324,7 @@
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E84" s="4">
         <v>3430</v>
@@ -8335,10 +8333,10 @@
         <v>231</v>
       </c>
       <c r="G84" s="8" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H84" s="10" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="I84" s="4" t="s">
         <v>113</v>
@@ -8364,7 +8362,7 @@
       </c>
       <c r="Q84" s="3"/>
       <c r="R84" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="S84" s="6" t="s">
         <v>224</v>
@@ -8379,7 +8377,7 @@
         <v>225</v>
       </c>
       <c r="W84" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X84" s="3">
         <v>0</v>
@@ -8388,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:1019" s="7" customFormat="1" ht="146.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:1019" s="7" customFormat="1" ht="146.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="3" t="s">
         <v>84</v>
       </c>
@@ -8397,7 +8395,7 @@
       </c>
       <c r="C85" s="3"/>
       <c r="D85" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E85" s="4">
         <v>3440</v>
@@ -8406,10 +8404,10 @@
         <v>213</v>
       </c>
       <c r="G85" s="8" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H85" s="10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I85" s="4" t="s">
         <v>113</v>
@@ -8435,7 +8433,7 @@
       </c>
       <c r="Q85" s="3"/>
       <c r="R85" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="S85" s="6" t="s">
         <v>224</v>
@@ -8450,7 +8448,7 @@
         <v>225</v>
       </c>
       <c r="W85" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X85" s="3">
         <v>0</v>
@@ -8459,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:1019" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:1019" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="3" t="s">
         <v>86</v>
       </c>
@@ -8474,13 +8472,13 @@
         <v>3450</v>
       </c>
       <c r="F86" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="G86" s="8" t="s">
+        <v>570</v>
+      </c>
+      <c r="H86" s="10" t="s">
         <v>549</v>
-      </c>
-      <c r="G86" s="8" t="s">
-        <v>571</v>
-      </c>
-      <c r="H86" s="10" t="s">
-        <v>550</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>113</v>
@@ -8506,7 +8504,7 @@
       </c>
       <c r="Q86" s="3"/>
       <c r="R86" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="S86" s="6" t="s">
         <v>224</v>
@@ -8521,7 +8519,7 @@
         <v>225</v>
       </c>
       <c r="W86" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X86" s="3">
         <v>0</v>
@@ -8530,7 +8528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:1019" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:1019" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="3" t="s">
         <v>86</v>
       </c>
@@ -8545,13 +8543,13 @@
         <v>3460</v>
       </c>
       <c r="F87" s="17" t="s">
+        <v>550</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>571</v>
+      </c>
+      <c r="H87" s="10" t="s">
         <v>551</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>572</v>
-      </c>
-      <c r="H87" s="10" t="s">
-        <v>552</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>113</v>
@@ -8577,7 +8575,7 @@
       </c>
       <c r="Q87" s="3"/>
       <c r="R87" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="S87" s="6" t="s">
         <v>224</v>
@@ -8592,7 +8590,7 @@
         <v>225</v>
       </c>
       <c r="W87" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X87" s="3">
         <v>0</v>
@@ -8601,7 +8599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:1019" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:1019" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="3" t="s">
         <v>86</v>
       </c>
@@ -8616,13 +8614,13 @@
         <v>3470</v>
       </c>
       <c r="F88" s="16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="G88" s="8" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H88" s="10" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I88" s="4" t="s">
         <v>113</v>
@@ -8648,7 +8646,7 @@
       </c>
       <c r="Q88" s="3"/>
       <c r="R88" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S88" s="6" t="s">
         <v>224</v>
@@ -8663,7 +8661,7 @@
         <v>225</v>
       </c>
       <c r="W88" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X88" s="3">
         <v>0</v>
@@ -8672,7 +8670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:1019" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:1019" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="3" t="s">
         <v>84</v>
       </c>
@@ -8690,10 +8688,10 @@
         <v>73</v>
       </c>
       <c r="G89" s="8" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H89" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I89" s="4" t="s">
         <v>113</v>
@@ -8711,7 +8709,7 @@
         <v>999999</v>
       </c>
       <c r="N89" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O89" s="3"/>
       <c r="P89" s="3">
@@ -8719,7 +8717,7 @@
       </c>
       <c r="Q89" s="3"/>
       <c r="R89" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S89" s="6" t="s">
         <v>224</v>
@@ -8734,7 +8732,7 @@
         <v>225</v>
       </c>
       <c r="W89" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X89" s="3">
         <v>0</v>
@@ -9737,7 +9735,7 @@
       <c r="AMD89"/>
       <c r="AME89"/>
     </row>
-    <row r="90" spans="1:1019" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:1019" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="3" t="s">
         <v>84</v>
       </c>
@@ -9755,10 +9753,10 @@
         <v>74</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H90" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I90" s="4" t="s">
         <v>113</v>
@@ -9776,7 +9774,7 @@
         <v>999999</v>
       </c>
       <c r="N90" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O90" s="3"/>
       <c r="P90" s="3">
@@ -9784,7 +9782,7 @@
       </c>
       <c r="Q90" s="3"/>
       <c r="R90" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="S90" s="6" t="s">
         <v>224</v>
@@ -9799,7 +9797,7 @@
         <v>225</v>
       </c>
       <c r="W90" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X90" s="3">
         <v>0</v>
@@ -9808,7 +9806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:1019" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:1019" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="3" t="s">
         <v>84</v>
       </c>
@@ -9826,10 +9824,10 @@
         <v>75</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>113</v>
@@ -9847,7 +9845,7 @@
         <v>999999</v>
       </c>
       <c r="N91" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O91" s="3"/>
       <c r="P91" s="3">
@@ -9855,7 +9853,7 @@
       </c>
       <c r="Q91" s="3"/>
       <c r="R91" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="S91" s="6" t="s">
         <v>224</v>
@@ -9870,7 +9868,7 @@
         <v>225</v>
       </c>
       <c r="W91" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X91" s="3">
         <v>0</v>
@@ -9879,7 +9877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="3" t="s">
         <v>84</v>
       </c>
@@ -9897,10 +9895,10 @@
         <v>76</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I92" s="4" t="s">
         <v>113</v>
@@ -9918,7 +9916,7 @@
         <v>999999</v>
       </c>
       <c r="N92" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O92" s="3"/>
       <c r="P92" s="3">
@@ -9926,7 +9924,7 @@
       </c>
       <c r="Q92" s="3"/>
       <c r="R92" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="S92" s="6" t="s">
         <v>224</v>
@@ -9941,7 +9939,7 @@
         <v>225</v>
       </c>
       <c r="W92" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X92" s="3">
         <v>0</v>
@@ -9950,7 +9948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:1019" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:1019" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="3" t="s">
         <v>84</v>
       </c>
@@ -9968,10 +9966,10 @@
         <v>77</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H93" s="10" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>113</v>
@@ -9989,7 +9987,7 @@
         <v>999999</v>
       </c>
       <c r="N93" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O93" s="3"/>
       <c r="P93" s="3">
@@ -9997,7 +9995,7 @@
       </c>
       <c r="Q93" s="3"/>
       <c r="R93" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="S93" s="6" t="s">
         <v>224</v>
@@ -10012,7 +10010,7 @@
         <v>225</v>
       </c>
       <c r="W93" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X93" s="3">
         <v>0</v>
@@ -10021,7 +10019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:1019" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:1019" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="3" t="s">
         <v>84</v>
       </c>
@@ -10039,10 +10037,10 @@
         <v>78</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H94" s="10" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I94" s="4" t="s">
         <v>113</v>
@@ -10060,7 +10058,7 @@
         <v>999999</v>
       </c>
       <c r="N94" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O94" s="3"/>
       <c r="P94" s="3">
@@ -10068,7 +10066,7 @@
       </c>
       <c r="Q94" s="3"/>
       <c r="R94" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="S94" s="6" t="s">
         <v>224</v>
@@ -10083,7 +10081,7 @@
         <v>225</v>
       </c>
       <c r="W94" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X94" s="3">
         <v>0</v>
@@ -10092,7 +10090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:1019" s="7" customFormat="1" ht="146.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:1019" s="7" customFormat="1" ht="146.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="3" t="s">
         <v>84</v>
       </c>
@@ -10110,10 +10108,10 @@
         <v>79</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H95" s="10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I95" s="4" t="s">
         <v>113</v>
@@ -10131,7 +10129,7 @@
         <v>999999</v>
       </c>
       <c r="N95" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O95" s="3"/>
       <c r="P95" s="3">
@@ -10139,7 +10137,7 @@
       </c>
       <c r="Q95" s="3"/>
       <c r="R95" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="S95" s="6" t="s">
         <v>224</v>
@@ -10154,7 +10152,7 @@
         <v>225</v>
       </c>
       <c r="W95" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X95" s="3">
         <v>0</v>
@@ -10163,7 +10161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:1019" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:1019" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="3" t="s">
         <v>84</v>
       </c>
@@ -10181,10 +10179,10 @@
         <v>80</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>113</v>
@@ -10202,7 +10200,7 @@
         <v>999999</v>
       </c>
       <c r="N96" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O96" s="3"/>
       <c r="P96" s="3">
@@ -10210,7 +10208,7 @@
       </c>
       <c r="Q96" s="3"/>
       <c r="R96" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="S96" s="6" t="s">
         <v>224</v>
@@ -10225,7 +10223,7 @@
         <v>225</v>
       </c>
       <c r="W96" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X96" s="3">
         <v>0</v>
@@ -11228,7 +11226,7 @@
       <c r="AMD96" s="7"/>
       <c r="AME96" s="7"/>
     </row>
-    <row r="97" spans="1:25" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:25" s="7" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="3" t="s">
         <v>84</v>
       </c>
@@ -11247,7 +11245,7 @@
       </c>
       <c r="G97" s="19"/>
       <c r="H97" s="10" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>113</v>
@@ -11265,7 +11263,7 @@
         <v>999999</v>
       </c>
       <c r="N97" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O97" s="3"/>
       <c r="P97" s="3">
@@ -11273,7 +11271,7 @@
       </c>
       <c r="Q97" s="3"/>
       <c r="R97" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="S97" s="6" t="s">
         <v>224</v>
@@ -11288,7 +11286,7 @@
         <v>225</v>
       </c>
       <c r="W97" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X97" s="3">
         <v>0</v>
@@ -11297,7 +11295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="3" t="s">
         <v>86</v>
       </c>
@@ -11312,13 +11310,13 @@
         <v>4072</v>
       </c>
       <c r="F98" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="G98" s="8" t="s">
+        <v>569</v>
+      </c>
+      <c r="H98" s="10" t="s">
         <v>547</v>
-      </c>
-      <c r="G98" s="8" t="s">
-        <v>570</v>
-      </c>
-      <c r="H98" s="10" t="s">
-        <v>548</v>
       </c>
       <c r="I98" s="4" t="s">
         <v>113</v>
@@ -11336,7 +11334,7 @@
         <v>999999</v>
       </c>
       <c r="N98" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O98" s="3"/>
       <c r="P98" s="3">
@@ -11344,7 +11342,7 @@
       </c>
       <c r="Q98" s="3"/>
       <c r="R98" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="S98" s="3"/>
       <c r="T98" s="3">
@@ -11357,7 +11355,7 @@
         <v>225</v>
       </c>
       <c r="W98" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X98" s="3">
         <v>0</v>
@@ -11366,7 +11364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:25" s="7" customFormat="1" ht="67.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:25" s="7" customFormat="1" ht="67.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="3" t="s">
         <v>84</v>
       </c>
@@ -11381,13 +11379,13 @@
         <v>4080</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H99" s="10" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I99" s="4" t="s">
         <v>113</v>
@@ -11405,7 +11403,7 @@
         <v>999999</v>
       </c>
       <c r="N99" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O99" s="3"/>
       <c r="P99" s="3">
@@ -11413,7 +11411,7 @@
       </c>
       <c r="Q99" s="3"/>
       <c r="R99" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="S99" s="6" t="s">
         <v>224</v>
@@ -11428,7 +11426,7 @@
         <v>225</v>
       </c>
       <c r="W99" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X99" s="3">
         <v>0</v>
@@ -11437,7 +11435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:25" s="7" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:25" s="7" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="3" t="s">
         <v>84</v>
       </c>
@@ -11455,10 +11453,10 @@
         <v>81</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H100" s="10" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I100" s="4" t="s">
         <v>113</v>
@@ -11476,7 +11474,7 @@
         <v>999999</v>
       </c>
       <c r="N100" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O100" s="3"/>
       <c r="P100" s="3">
@@ -11484,7 +11482,7 @@
       </c>
       <c r="Q100" s="3"/>
       <c r="R100" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="S100" s="6" t="s">
         <v>224</v>
@@ -11499,7 +11497,7 @@
         <v>225</v>
       </c>
       <c r="W100" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X100" s="3">
         <v>0</v>
@@ -11526,10 +11524,10 @@
         <v>82</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I101" s="4" t="s">
         <v>113</v>
@@ -11555,7 +11553,7 @@
       </c>
       <c r="Q101" s="3"/>
       <c r="R101" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="S101" s="6" t="s">
         <v>224</v>
@@ -11570,7 +11568,7 @@
         <v>225</v>
       </c>
       <c r="W101" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X101" s="3">
         <v>0</v>
@@ -11579,7 +11577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:25" s="7" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:25" s="7" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="3" t="s">
         <v>84</v>
       </c>
@@ -11597,10 +11595,10 @@
         <v>83</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H102" s="10" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I102" s="4" t="s">
         <v>113</v>
@@ -11618,7 +11616,7 @@
         <v>999999</v>
       </c>
       <c r="N102" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O102" s="3"/>
       <c r="P102" s="3">
@@ -11626,7 +11624,7 @@
       </c>
       <c r="Q102" s="3"/>
       <c r="R102" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="S102" s="6" t="s">
         <v>224</v>
@@ -11641,7 +11639,7 @@
         <v>225</v>
       </c>
       <c r="W102" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X102" s="3">
         <v>0</v>
@@ -11650,7 +11648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:25" s="7" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:25" s="7" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="3" t="s">
         <v>84</v>
       </c>
@@ -11659,19 +11657,19 @@
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E103" s="4">
         <v>4120</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H103" s="10" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I103" s="4" t="s">
         <v>113</v>
@@ -11697,7 +11695,7 @@
       </c>
       <c r="Q103" s="3"/>
       <c r="R103" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="S103" s="6" t="s">
         <v>224</v>
@@ -11712,7 +11710,7 @@
         <v>225</v>
       </c>
       <c r="W103" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X103" s="3">
         <v>0</v>
@@ -11721,7 +11719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:25" s="7" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:25" s="7" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="3" t="s">
         <v>86</v>
       </c>
@@ -11730,19 +11728,19 @@
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E104" s="4">
         <v>4130</v>
       </c>
       <c r="F104" s="17" t="s">
+        <v>552</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="H104" s="10" t="s">
         <v>553</v>
-      </c>
-      <c r="G104" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="H104" s="10" t="s">
-        <v>554</v>
       </c>
       <c r="I104" s="4" t="s">
         <v>113</v>
@@ -11768,7 +11766,7 @@
       </c>
       <c r="Q104" s="3"/>
       <c r="R104" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="S104" s="3"/>
       <c r="T104" s="3">
@@ -11781,7 +11779,7 @@
         <v>225</v>
       </c>
       <c r="W104" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X104" s="3">
         <v>0</v>
@@ -11790,7 +11788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:25" s="7" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:25" s="7" customFormat="1" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="3" t="s">
         <v>92</v>
       </c>
@@ -11808,10 +11806,10 @@
         <v>23</v>
       </c>
       <c r="G105" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I105" s="4" t="s">
         <v>113</v>
@@ -11837,7 +11835,7 @@
       </c>
       <c r="Q105" s="3"/>
       <c r="R105" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="S105" s="6" t="s">
         <v>224</v>
@@ -11852,7 +11850,7 @@
         <v>225</v>
       </c>
       <c r="W105" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X105" s="3">
         <v>0</v>
@@ -11861,7 +11859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:25" s="7" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:25" s="7" customFormat="1" ht="49.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="3" t="s">
         <v>92</v>
       </c>
@@ -11879,10 +11877,10 @@
         <v>24</v>
       </c>
       <c r="G106" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I106" s="4" t="s">
         <v>113</v>
@@ -11908,7 +11906,7 @@
       </c>
       <c r="Q106" s="3"/>
       <c r="R106" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="S106" s="6" t="s">
         <v>224</v>
@@ -11923,7 +11921,7 @@
         <v>225</v>
       </c>
       <c r="W106" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X106" s="3">
         <v>0</v>
@@ -11932,7 +11930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:25" s="18" customFormat="1" ht="83.25" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:25" s="18" customFormat="1" ht="83.25" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="3" t="s">
         <v>92</v>
       </c>
@@ -11947,13 +11945,13 @@
         <v>5010</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G107" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I107" s="4" t="s">
         <v>113</v>
@@ -11979,7 +11977,7 @@
       </c>
       <c r="Q107" s="3"/>
       <c r="R107" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="S107" s="6" t="s">
         <v>224</v>
@@ -11994,7 +11992,7 @@
         <v>225</v>
       </c>
       <c r="W107" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X107" s="3">
         <v>0</v>
@@ -12003,7 +12001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:25" s="18" customFormat="1" ht="130.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:25" s="18" customFormat="1" ht="130.5" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="3" t="s">
         <v>92</v>
       </c>
@@ -12021,10 +12019,10 @@
         <v>26</v>
       </c>
       <c r="G108" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H108" s="10" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I108" s="4" t="s">
         <v>113</v>
@@ -12050,7 +12048,7 @@
       </c>
       <c r="Q108" s="3"/>
       <c r="R108" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="S108" s="6" t="s">
         <v>224</v>
@@ -12065,7 +12063,7 @@
         <v>225</v>
       </c>
       <c r="W108" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X108" s="3">
         <v>0</v>
@@ -12074,7 +12072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:25" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:25" s="18" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="3" t="s">
         <v>92</v>
       </c>
@@ -12092,10 +12090,10 @@
         <v>106</v>
       </c>
       <c r="G109" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H109" s="10" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I109" s="4" t="s">
         <v>113</v>
@@ -12121,7 +12119,7 @@
       </c>
       <c r="Q109" s="3"/>
       <c r="R109" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="S109" s="6" t="s">
         <v>224</v>
@@ -12136,7 +12134,7 @@
         <v>225</v>
       </c>
       <c r="W109" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X109" s="3">
         <v>0</v>
@@ -12145,7 +12143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:25" s="18" customFormat="1" ht="51.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:25" s="18" customFormat="1" ht="51.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="3" t="s">
         <v>92</v>
       </c>
@@ -12163,10 +12161,10 @@
         <v>25</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H110" s="10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I110" s="4" t="s">
         <v>113</v>
@@ -12192,7 +12190,7 @@
       </c>
       <c r="Q110" s="3"/>
       <c r="R110" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="S110" s="6" t="s">
         <v>224</v>
@@ -12207,7 +12205,7 @@
         <v>225</v>
       </c>
       <c r="W110" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X110" s="3">
         <v>0</v>
@@ -12216,7 +12214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:25" s="18" customFormat="1" ht="114.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:25" s="18" customFormat="1" ht="114.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="3" t="s">
         <v>92</v>
       </c>
@@ -12234,10 +12232,10 @@
         <v>21</v>
       </c>
       <c r="G111" s="8" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H111" s="10" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I111" s="4" t="s">
         <v>113</v>
@@ -12263,7 +12261,7 @@
       </c>
       <c r="Q111" s="3"/>
       <c r="R111" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="S111" s="6" t="s">
         <v>224</v>
@@ -12278,7 +12276,7 @@
         <v>225</v>
       </c>
       <c r="W111" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X111" s="3">
         <v>0</v>
@@ -12287,7 +12285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:25" s="18" customFormat="1" ht="99" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:25" s="18" customFormat="1" ht="99" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="3" t="s">
         <v>92</v>
       </c>
@@ -12305,10 +12303,10 @@
         <v>22</v>
       </c>
       <c r="G112" s="8" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H112" s="10" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="I112" s="4" t="s">
         <v>113</v>
@@ -12334,7 +12332,7 @@
       </c>
       <c r="Q112" s="3"/>
       <c r="R112" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="S112" s="6" t="s">
         <v>224</v>
@@ -12349,7 +12347,7 @@
         <v>225</v>
       </c>
       <c r="W112" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X112" s="3">
         <v>0</v>
@@ -12358,7 +12356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:25" s="18" customFormat="1" ht="51.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:25" s="18" customFormat="1" ht="51.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="3" t="s">
         <v>221</v>
       </c>
@@ -12376,10 +12374,10 @@
         <v>215</v>
       </c>
       <c r="G113" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H113" s="10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I113" s="4" t="s">
         <v>113</v>
@@ -12405,7 +12403,7 @@
       </c>
       <c r="Q113" s="3"/>
       <c r="R113" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="S113" s="6" t="s">
         <v>224</v>
@@ -12420,7 +12418,7 @@
         <v>225</v>
       </c>
       <c r="W113" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X113" s="3">
         <v>0</v>
@@ -12429,7 +12427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:25" s="18" customFormat="1" ht="51.75" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:25" s="18" customFormat="1" ht="51.75" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="3" t="s">
         <v>221</v>
       </c>
@@ -12447,10 +12445,10 @@
         <v>216</v>
       </c>
       <c r="G114" s="8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H114" s="10" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="I114" s="4" t="s">
         <v>113</v>
@@ -12476,7 +12474,7 @@
       </c>
       <c r="Q114" s="3"/>
       <c r="R114" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="S114" s="6" t="s">
         <v>224</v>
@@ -12491,7 +12489,7 @@
         <v>225</v>
       </c>
       <c r="W114" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="X114" s="3">
         <v>0</v>
@@ -12501,6 +12499,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Y114">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="pouch"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:Y115">
     <sortCondition ref="E2:E115"/>
   </sortState>

</xml_diff>